<commit_message>
upadted investigation in pseudoArc
</commit_message>
<xml_diff>
--- a/Mitochondria in Hela Cells/pseudoARC/isa.investigation.xlsx
+++ b/Mitochondria in Hela Cells/pseudoARC/isa.investigation.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Schauss-Lab\Datamanagement\NFDI\ISA Beispiele EM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Schauss-Lab\Datamanagement\NFDI\ISA Beispiele EM\omero-arc-testdata\Mitochondria in Hela Cells\pseudoARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CF96E5-A192-404B-838A-97BBB6C4EC57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BFC0A6-5327-44ED-9AF1-9BCE9F10B105}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="315" yWindow="375" windowWidth="38025" windowHeight="17805" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
+    <workbookView xWindow="315" yWindow="375" windowWidth="38025" windowHeight="17805" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_investigation" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="151">
   <si>
     <t>ONTOLOGY SOURCE REFERENCE</t>
   </si>
@@ -414,13 +414,73 @@
   </si>
   <si>
     <t>https://orcid.org/0000-0002-7744-4940</t>
+  </si>
+  <si>
+    <t>OBI</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/obi.owl</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/obi/2023-09-20/obi.owl</t>
+  </si>
+  <si>
+    <t>Ontology for Biomedical Investigations</t>
+  </si>
+  <si>
+    <t>CHMO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/chmo.owl</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/chmo/releases/2022-04-19/chmo.owl</t>
+  </si>
+  <si>
+    <t>Chemical Methods Ontology</t>
+  </si>
+  <si>
+    <t>DPBO</t>
+  </si>
+  <si>
+    <t>UO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/uo.owl</t>
+  </si>
+  <si>
+    <t>Units of measurement ontology</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/uo/releases/2023-05-25/uo.owl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/nfdi4plants/nfdi4plants_ontology/main/dpbo.obo</t>
+  </si>
+  <si>
+    <t>init/2020-12-01</t>
+  </si>
+  <si>
+    <t>DataPLANT biology ontology</t>
+  </si>
+  <si>
+    <t>https://gitlab.com/openmicroscopy/incubator/ome-owl/-/blob/bd02745587446276cbce5e3f6d2e8fef76530f57/ontology/owl/ome_core/ome_core.owl.ttl</t>
+  </si>
+  <si>
+    <t>OME data model core ontology</t>
+  </si>
+  <si>
+    <t>OME-core</t>
+  </si>
+  <si>
+    <t>2016-06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -568,6 +628,11 @@
       <color rgb="FFCCCCCC"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="33">
@@ -912,12 +977,19 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1274,28 +1346,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="101.625" customWidth="1"/>
-    <col min="3" max="3" width="255.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="198" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="47.625" customWidth="1"/>
+    <col min="4" max="4" width="42.375" customWidth="1"/>
+    <col min="5" max="5" width="60.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.875" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1305,8 +1379,24 @@
       <c r="C2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1316,8 +1406,23 @@
       <c r="C3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1327,8 +1432,23 @@
       <c r="C4" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1338,13 +1458,28 @@
       <c r="C5" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1352,7 +1487,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1360,15 +1495,16 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1376,17 +1512,17 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1394,7 +1530,7 @@
         <v>36344526</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1402,7 +1538,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1410,7 +1546,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1967,9 +2103,10 @@
     <hyperlink ref="B86" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B32" r:id="rId3" xr:uid="{50F7E1EF-272C-4552-B82A-04FE9854DFF7}"/>
     <hyperlink ref="C32" r:id="rId4" xr:uid="{B40E6101-5B03-4A63-807A-049137905FFF}"/>
+    <hyperlink ref="F3" r:id="rId5" xr:uid="{6954CEA1-9213-4FCF-AB99-1D6645E5A432}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>